<commit_message>
edit and save timesheet functionality
</commit_message>
<xml_diff>
--- a/EmployeeTimesheet.xlsx
+++ b/EmployeeTimesheet.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
   <si>
     <t>Client Manager Name</t>
   </si>
@@ -90,25 +90,16 @@
     <t>29-Jul</t>
   </si>
   <si>
-    <t xml:space="preserve">Testing ( 1 ) </t>
+    <t xml:space="preserve">Development ( 1 ) </t>
+  </si>
+  <si>
+    <t>11</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t xml:space="preserve">Client call ( 1 ) </t>
-  </si>
-  <si>
     <t>17</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>132</t>
   </si>
   <si>
     <t>Offshore Consultant's Project Manager's Name :dhananjayKumar@gmail.com</t>
@@ -1163,53 +1154,37 @@
         <v>22</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L9" s="9"/>
     </row>
     <row r="10" spans="1:12" ht="42.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
-      <c r="B10" s="12" t="s">
-        <v>23</v>
-      </c>
+      <c r="B10" s="12"/>
       <c r="C10" s="13"/>
       <c r="D10" s="11"/>
-      <c r="E10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J10" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="K10" s="11" t="s">
-        <v>25</v>
-      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
       <c r="L10" s="11"/>
     </row>
     <row r="11" spans="1:12" ht="42.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -1317,25 +1292,25 @@
       <c r="C18" s="74"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="L18" s="10"/>
     </row>
@@ -1345,7 +1320,7 @@
       </c>
       <c r="C19" s="83"/>
       <c r="D19" s="84" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E19" s="84"/>
       <c r="F19" s="84"/>
@@ -1389,7 +1364,7 @@
         <v>6</v>
       </c>
       <c r="B22" s="62" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C22" s="63"/>
       <c r="D22" s="63"/>
@@ -1435,7 +1410,7 @@
         <v>0</v>
       </c>
       <c r="B25" s="53" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C25" s="54"/>
       <c r="D25" s="54"/>

</xml_diff>

<commit_message>
toggle button after generating excel sheet ie edit timesheet in place of save timesheet
</commit_message>
<xml_diff>
--- a/EmployeeTimesheet.xlsx
+++ b/EmployeeTimesheet.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
   <si>
     <t>Client Manager Name</t>
   </si>
@@ -66,37 +66,52 @@
     <t>Teach For America</t>
   </si>
   <si>
-    <t>7/23/2018-7/29/2018</t>
-  </si>
-  <si>
-    <t>23-Jul</t>
-  </si>
-  <si>
-    <t>24-Jul</t>
-  </si>
-  <si>
-    <t>25-Jul</t>
-  </si>
-  <si>
-    <t>26-Jul</t>
-  </si>
-  <si>
-    <t>27-Jul</t>
-  </si>
-  <si>
-    <t>28-Jul</t>
-  </si>
-  <si>
-    <t>29-Jul</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Client call ( 1 ) </t>
+    <t>7/2/2018-7/8/2018</t>
+  </si>
+  <si>
+    <t>2-Jul</t>
+  </si>
+  <si>
+    <t>3-Jul</t>
+  </si>
+  <si>
+    <t>4-Jul</t>
+  </si>
+  <si>
+    <t>5-Jul</t>
+  </si>
+  <si>
+    <t>6-Jul</t>
+  </si>
+  <si>
+    <t>7-Jul</t>
+  </si>
+  <si>
+    <t>8-Jul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing ( 1 ) </t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>7</t>
+    <t xml:space="preserve">Client call ( 12 ) </t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>45</t>
   </si>
   <si>
     <t>Offshore Consultant's Project Manager's Name :Dhananjay Kumar</t>
@@ -1172,16 +1187,32 @@
     </row>
     <row r="10" spans="1:12" ht="42.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
-      <c r="B10" s="12"/>
+      <c r="B10" s="12" t="s">
+        <v>23</v>
+      </c>
       <c r="C10" s="13"/>
       <c r="D10" s="11"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
+      <c r="E10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>22</v>
+      </c>
       <c r="L10" s="11"/>
     </row>
     <row r="11" spans="1:12" ht="42.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -1289,25 +1320,25 @@
       <c r="C18" s="74"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="L18" s="10"/>
     </row>
@@ -1317,7 +1348,7 @@
       </c>
       <c r="C19" s="83"/>
       <c r="D19" s="84" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E19" s="84"/>
       <c r="F19" s="84"/>
@@ -1361,7 +1392,7 @@
         <v>6</v>
       </c>
       <c r="B22" s="62" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C22" s="63"/>
       <c r="D22" s="63"/>
@@ -1407,7 +1438,7 @@
         <v>0</v>
       </c>
       <c r="B25" s="53" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C25" s="54"/>
       <c r="D25" s="54"/>

</xml_diff>

<commit_message>
changes in application properties as the data is in mongodb atlas
</commit_message>
<xml_diff>
--- a/EmployeeTimesheet.xlsx
+++ b/EmployeeTimesheet.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
   <si>
     <t>Client Manager Name</t>
   </si>
@@ -60,46 +60,49 @@
     <t>Total hours for the week</t>
   </si>
   <si>
-    <t>Tanuj Khaturia</t>
+    <t>Vineet Rajput</t>
   </si>
   <si>
     <t>Teach For America</t>
   </si>
   <si>
-    <t>10/8/2018-10/14/2018</t>
-  </si>
-  <si>
-    <t>8-Oct</t>
-  </si>
-  <si>
-    <t>9-Oct</t>
-  </si>
-  <si>
-    <t>10-Oct</t>
-  </si>
-  <si>
-    <t>11-Oct</t>
-  </si>
-  <si>
-    <t>12-Oct</t>
-  </si>
-  <si>
-    <t>13-Oct</t>
-  </si>
-  <si>
-    <t>14-Oct</t>
-  </si>
-  <si>
-    <t>Testing</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Offshore Consultant's Project Manager's Name :Dhananjay Kumar</t>
-  </si>
-  <si>
-    <t>Omar colon</t>
+    <t>7/23/2018-7/29/2018</t>
+  </si>
+  <si>
+    <t>23-Jul</t>
+  </si>
+  <si>
+    <t>24-Jul</t>
+  </si>
+  <si>
+    <t>25-Jul</t>
+  </si>
+  <si>
+    <t>26-Jul</t>
+  </si>
+  <si>
+    <t>27-Jul</t>
+  </si>
+  <si>
+    <t>28-Jul</t>
+  </si>
+  <si>
+    <t>29-Jul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Client Call ( sanchit ) </t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Offshore Consultant's Project Manager's Name :dhananjayKumar@gmail.com</t>
+  </si>
+  <si>
+    <t>Omarcolon@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1314,7 +1317,7 @@
       </c>
       <c r="C19" s="83"/>
       <c r="D19" s="84" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E19" s="84"/>
       <c r="F19" s="84"/>
@@ -1358,7 +1361,7 @@
         <v>6</v>
       </c>
       <c r="B22" s="62" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C22" s="63"/>
       <c r="D22" s="63"/>
@@ -1404,7 +1407,7 @@
         <v>0</v>
       </c>
       <c r="B25" s="53" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C25" s="54"/>
       <c r="D25" s="54"/>

</xml_diff>

<commit_message>
environment changes and new dist folder created.
</commit_message>
<xml_diff>
--- a/EmployeeTimesheet.xlsx
+++ b/EmployeeTimesheet.xlsx
@@ -60,37 +60,37 @@
     <t>Total hours for the week</t>
   </si>
   <si>
-    <t>Vineet Rajput</t>
+    <t>Tanuj Khaturia</t>
   </si>
   <si>
     <t>Teach For America</t>
   </si>
   <si>
-    <t>7/23/2018-7/29/2018</t>
-  </si>
-  <si>
-    <t>23-Jul</t>
-  </si>
-  <si>
-    <t>24-Jul</t>
-  </si>
-  <si>
-    <t>25-Jul</t>
-  </si>
-  <si>
-    <t>26-Jul</t>
-  </si>
-  <si>
-    <t>27-Jul</t>
-  </si>
-  <si>
-    <t>28-Jul</t>
-  </si>
-  <si>
-    <t>29-Jul</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Client Call ( sanchit ) </t>
+    <t>7/30/2018-8/5/2018</t>
+  </si>
+  <si>
+    <t>30-Jul</t>
+  </si>
+  <si>
+    <t>31-Jul</t>
+  </si>
+  <si>
+    <t>1-Aug</t>
+  </si>
+  <si>
+    <t>2-Aug</t>
+  </si>
+  <si>
+    <t>3-Aug</t>
+  </si>
+  <si>
+    <t>4-Aug</t>
+  </si>
+  <si>
+    <t>5-Aug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Client Call ( 1 ) </t>
   </si>
   <si>
     <t>1</t>

</xml_diff>